<commit_message>
Can now have any number of aggregate_difficulty rounds. Was limited to just 1 before.
</commit_message>
<xml_diff>
--- a/quiz_metadata.xlsx
+++ b/quiz_metadata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="12">
   <si>
     <t xml:space="preserve">Question</t>
   </si>
@@ -43,19 +43,19 @@
     <t xml:space="preserve">aggregate_difficulty</t>
   </si>
   <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
     <t xml:space="preserve">D</t>
   </si>
   <si>
     <t xml:space="preserve">C</t>
   </si>
   <si>
-    <t xml:space="preserve">B</t>
+    <t xml:space="preserve">3.10</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.10</t>
   </si>
 </sst>
 </file>
@@ -176,15 +176,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -272,114 +273,183 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="4" t="n">
         <v>2.1</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="4" t="n">
         <v>2.2</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="3" t="s">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="3" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="3" t="s">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="3" t="s">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="0" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
-        <v>2.9</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>9</v>
-      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Reorganized functions relating to final scoring and aggregate difficulty round scoring
</commit_message>
<xml_diff>
--- a/quiz_metadata.xlsx
+++ b/quiz_metadata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
   <si>
     <t xml:space="preserve">Question</t>
   </si>
@@ -38,24 +38,6 @@
   </si>
   <si>
     <t xml:space="preserve">A,B,C,D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aggregate_difficulty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
   </si>
 </sst>
 </file>
@@ -179,10 +161,10 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.16"/>
@@ -273,180 +255,52 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>7</v>
-      </c>
+      <c r="A9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>7</v>
-      </c>
+      <c r="A10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>8</v>
-      </c>
+      <c r="A11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>9</v>
-      </c>
+      <c r="A12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>7</v>
-      </c>
+      <c r="A13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="n">
-        <v>2.6</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>9</v>
-      </c>
+      <c r="A14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="n">
-        <v>2.7</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>9</v>
-      </c>
+      <c r="A15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>8</v>
-      </c>
+      <c r="A16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="n">
-        <v>2.9</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>7</v>
-      </c>
+      <c r="A17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>8</v>
-      </c>
+      <c r="A18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>9</v>
-      </c>
+      <c r="A19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>7</v>
-      </c>
+      <c r="A20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>11</v>
-      </c>
+      <c r="A21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="n">
-        <v>3.4</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>8</v>
-      </c>
+      <c r="A22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>8</v>
-      </c>
+      <c r="A23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>11</v>
-      </c>
+      <c r="A24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>

</xml_diff>

<commit_message>
Added text_logic for text rounds. Added Custom_scoring to metadata
</commit_message>
<xml_diff>
--- a/quiz_metadata.xlsx
+++ b/quiz_metadata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="14">
   <si>
     <t xml:space="preserve">Question</t>
   </si>
@@ -31,13 +31,37 @@
     <t xml:space="preserve">Valid_answers</t>
   </si>
   <si>
+    <t xml:space="preserve">Custom_scoring</t>
+  </si>
+  <si>
     <t xml:space="preserve">text</t>
   </si>
   <si>
+    <t xml:space="preserve">TON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUEUE</t>
+  </si>
+  <si>
     <t xml:space="preserve">least_popular</t>
   </si>
   <si>
     <t xml:space="preserve">A,B,C,D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aggregate_difficulty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A</t>
   </si>
 </sst>
 </file>
@@ -158,15 +182,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.16"/>
   </cols>
   <sheetData>
@@ -180,34 +204,47 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
         <v>0.1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
         <v>0.2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>1.1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -215,10 +252,10 @@
         <v>1.2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -226,10 +263,10 @@
         <v>1.3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -237,10 +274,10 @@
         <v>1.4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -248,56 +285,176 @@
         <v>1.5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4"/>
+      <c r="A9" s="4" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4"/>
+      <c r="A10" s="4" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4"/>
+      <c r="A11" s="4" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4"/>
+      <c r="A12" s="4" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4"/>
+      <c r="A13" s="4" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4"/>
+      <c r="A14" s="4" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4"/>
+      <c r="A15" s="4" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4"/>
+      <c r="A16" s="4" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4"/>
+      <c r="A17" s="4" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4"/>
+      <c r="A18" s="4" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4"/>
+      <c r="A19" s="4" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4"/>
+      <c r="A20" s="4" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4"/>
+      <c r="A21" s="4" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4"/>
+      <c r="A22" s="4" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4"/>
+      <c r="A23" s="4" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>

</xml_diff>

<commit_message>
Added functions to validate player answer sheets and quiz metadata inputs
</commit_message>
<xml_diff>
--- a/quiz_metadata.xlsx
+++ b/quiz_metadata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
   <si>
     <t xml:space="preserve">Question</t>
   </si>
@@ -49,19 +49,31 @@
     <t xml:space="preserve">A,B,C,D</t>
   </si>
   <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">aggregate_difficulty</t>
   </si>
   <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
     <t xml:space="preserve">B</t>
   </si>
   <si>
     <t xml:space="preserve">D</t>
   </si>
   <si>
+    <t xml:space="preserve">2.4</t>
+  </si>
+  <si>
     <t xml:space="preserve">C</t>
   </si>
   <si>
-    <t xml:space="preserve">A</t>
+    <t xml:space="preserve">2.10</t>
   </si>
 </sst>
 </file>
@@ -185,10 +197,10 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4609375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.47265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.16"/>
@@ -246,10 +258,13 @@
       <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="D4" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
-        <v>1.2</v>
+      <c r="A5" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
@@ -296,10 +311,10 @@
         <v>2.1</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -307,10 +322,10 @@
         <v>2.2</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -318,21 +333,21 @@
         <v>2.3</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="n">
-        <v>2.4</v>
+      <c r="A12" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -340,10 +355,10 @@
         <v>2.5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -351,10 +366,10 @@
         <v>2.6</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -362,10 +377,10 @@
         <v>2.7</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -373,10 +388,10 @@
         <v>2.8</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -384,40 +399,40 @@
         <v>2.9</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="n">
-        <v>3.1</v>
+      <c r="A18" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="n">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="n">
-        <v>3.3</v>
+        <v>3.2</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>13</v>
@@ -425,39 +440,47 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="n">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="n">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="n">
         <v>3.6</v>
       </c>
-      <c r="B23" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0"/>
+      <c r="B24" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>

</xml_diff>

<commit_message>
Added lock_answers function to prevent players from cheating
</commit_message>
<xml_diff>
--- a/quiz_metadata.xlsx
+++ b/quiz_metadata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="17">
   <si>
     <t xml:space="preserve">Question</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t xml:space="preserve">A,B,C,D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a</t>
   </si>
   <si>
     <t xml:space="preserve">1.2</t>
@@ -197,7 +194,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.47265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -258,13 +255,10 @@
       <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
@@ -311,10 +305,10 @@
         <v>2.1</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -322,10 +316,10 @@
         <v>2.2</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -333,21 +327,21 @@
         <v>2.3</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -355,10 +349,10 @@
         <v>2.5</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -366,10 +360,10 @@
         <v>2.6</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -377,10 +371,10 @@
         <v>2.7</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -388,10 +382,10 @@
         <v>2.8</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -399,21 +393,21 @@
         <v>2.9</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -421,10 +415,10 @@
         <v>3.1</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -432,10 +426,10 @@
         <v>3.2</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -443,10 +437,10 @@
         <v>3.3</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -454,10 +448,10 @@
         <v>3.4</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -465,10 +459,10 @@
         <v>3.5</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -476,10 +470,10 @@
         <v>3.6</v>
       </c>
       <c r="B24" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>